<commit_message>
feat(Proveedores - Solicitudes de precio): Visualizadas últimas 3 compras
</commit_message>
<xml_diff>
--- a/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
+++ b/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\application\views\reportes\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8542F6-A20E-4CA4-A5F3-B48451C75076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF4B99B-FE03-438C-A420-D8D1AB8C26A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AB0910D4-337B-4AA8-B272-A0A042017033}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB0910D4-337B-4AA8-B272-A0A042017033}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>CENTRO DE OPERACIÓN</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>MONEDA DOCTO</t>
+  </si>
+  <si>
+    <t>COMPRAS ANTERIORES</t>
   </si>
 </sst>
 </file>
@@ -186,8 +189,14 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Moneda 2" xfId="1" xr:uid="{A22D5077-FF25-4BB0-A127-7667B8A7F084}"/>
@@ -534,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4220408-FBA5-4CB2-8B37-E5540C6C2A2C}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -582,11 +591,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3254C59D-5EEE-4ABA-B049-38AD83484C92}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -603,42 +610,50 @@
     <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor(Proveedores - Solicitudes - Órdenes Excel): Agregadas observaciones
</commit_message>
<xml_diff>
--- a/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
+++ b/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\application\views\reportes\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF4B99B-FE03-438C-A420-D8D1AB8C26A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5A704-6AEB-4D3F-BCE3-5CCF359045BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB0910D4-337B-4AA8-B272-A0A042017033}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>CENTRO DE OPERACIÓN</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>COMPRAS ANTERIORES</t>
+  </si>
+  <si>
+    <t>OBSERVACIÓN</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3254C59D-5EEE-4ABA-B049-38AD83484C92}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
@@ -608,9 +611,10 @@
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,6 +653,9 @@
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat(Proveedores - Orden compra Excel): Muestra nombre del último proveedor
</commit_message>
<xml_diff>
--- a/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
+++ b/application/views/reportes/plantillas/proveedores_orden_compra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectos\simon-bolivar\application\views\reportes\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5A704-6AEB-4D3F-BCE3-5CCF359045BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB556FA7-3994-433C-8901-D43915A2BF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB0910D4-337B-4AA8-B272-A0A042017033}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>CENTRO DE OPERACIÓN</t>
   </si>
@@ -61,9 +61,6 @@
     <t>COND. PAGO (P30, P45)</t>
   </si>
   <si>
-    <t>Tipo docto (FOC)</t>
-  </si>
-  <si>
     <t>CONSECUTIVO (LÍNEAS DE EXCEL)</t>
   </si>
   <si>
@@ -95,6 +92,12 @@
   </si>
   <si>
     <t>OBSERVACIÓN</t>
+  </si>
+  <si>
+    <t>PROVEEDOR ÚLTIMA COMPRA</t>
+  </si>
+  <si>
+    <t>Tipo docto</t>
   </si>
 </sst>
 </file>
@@ -195,10 +198,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -583,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -594,66 +597,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3254C59D-5EEE-4ABA-B049-38AD83484C92}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>